<commit_message>
file updates and analysis update
</commit_message>
<xml_diff>
--- a/files/stat.xlsx
+++ b/files/stat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Desktop\frontend playground\69. Website\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D68C7EA-E8D8-4616-9668-B9F045C8F4F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD0CDA66-769E-4925-B37D-91AEC6FD94AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D58E2BEA-D26D-492A-88D8-74F75718F47E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{68F71244-C937-477E-B2AD-DFE79BC4A93B}"/>
   </bookViews>
   <sheets>
     <sheet name="Stat" sheetId="1" r:id="rId1"/>
@@ -41,30 +41,141 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
-    <t>Math</t>
+    <t>Stat</t>
   </si>
   <si>
     <t>resume planning</t>
   </si>
   <si>
-    <t>s/n</t>
+    <t>Probability and Statistics (Wasserman - All of Statistics)</t>
   </si>
   <si>
-    <t>term</t>
+    <t>Contents</t>
   </si>
   <si>
-    <t>remarks</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wasserman's All of Statistics (Probability):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1. Probability
+2. Random Variables</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3. Expectation
+4. Inequalities
+5. Convergence of random variables</t>
+    </r>
   </si>
   <si>
-    <t>remarks 2</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wasserman's All of Statistics (Inference):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+6. Models, statistical inference and learning
+7. Estimating the CDF and statistical functionals
+8. Bootstrapping
+9. Parametric inference
+10. Hypothesis testing 
+11. Bayesian inference
+12. Statistical decision theory</t>
+    </r>
   </si>
   <si>
-    <t>cat</t>
-  </si>
-  <si>
-    <t>Wasserman- probability</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wasserman's All of Statistics (Statistical Models and Methods):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+13. Linear and logistic regression
+14. Multivariate models
+15. Inference about independence
+16. Causal inference
+17. Directed graphs and conditional independence
+18. Undirected graphs
+19. Log-Linear models
+20. Nonparametric curve estimation
+21. Smoothing using orthogonal functions
+22. Classification
+23. Probability redux: stochastic processes
+24. Simulation (Monte Carlo and MCMC)</t>
+    </r>
   </si>
   <si>
     <t>sample spaces &amp; events</t>
@@ -2334,7 +2445,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">moment (physics)
+      <t xml:space="preserve">Moment (physics)
 </t>
     </r>
     <r>
@@ -2359,7 +2470,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Mgf:</t>
+Moment Generating Function:</t>
     </r>
     <r>
       <rPr>
@@ -2628,9 +2739,6 @@
     </r>
   </si>
   <si>
-    <t>Wasserman - statistical inference</t>
-  </si>
-  <si>
     <t>introduction to statistical inference</t>
   </si>
   <si>
@@ -2918,230 +3026,6 @@
       </rPr>
       <t>(0.5)). Denoted by T(F), the functional on F.</t>
     </r>
-  </si>
-  <si>
-    <t>fundamental concepts in inference</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>point estimation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-best guess of a quantity of interest. Parametric point estimate:
-ϴ hat = g(X1…Xn), a function of the RVs.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Unbiasness of PPE:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-E(ϴ hat) = ϴ. The expected value of the parametric point estimate equals the parameter. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Consistency of PPE:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-ϴ hat --P--&gt; ϴ</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>sampling distribution:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-distribution of ϴ hat (sampling distribution).</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Standard error:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-se(ϴ hat) = [V(ϴ hat)]</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0.5</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>MSE (mean squared error):</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Expected value of (Error from actual </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>ϴ)^2.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-confidence interval:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-a 1-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>α CI is interval Cn = (a,b) where a=a(x1..xn) &amp; b=b(x1..xn) such that Pϴ(ϴ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>∈Cn) &gt;= 1-α</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">estimating the CDF &amp; statistical functionals </t>
-  </si>
-  <si>
-    <t>the bootstrap</t>
   </si>
   <si>
     <t>parametric inference</t>
@@ -3625,14 +3509,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3668,6 +3545,20 @@
       <u/>
       <sz val="16"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3872,15 +3763,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3892,10 +3783,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3904,11 +3795,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3917,30 +3805,30 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3969,13 +3857,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1388871</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>481853</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3983,7 +3871,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2882FA44-676E-4763-8415-A08A641E959E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B162DF49-94B1-4473-A5BB-5FC45526C37D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4005,7 +3893,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2714625" y="21802725"/>
+          <a:off x="2714625" y="24279225"/>
           <a:ext cx="1388871" cy="481853"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4019,13 +3907,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2943553</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>605117</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4033,7 +3921,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08E40D53-8035-4A47-9C04-7C1A858DDA3D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DD08F08-61E9-4E85-9E43-37E3A6C30B1A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4055,7 +3943,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5658178" y="21802725"/>
+          <a:off x="5658178" y="24279225"/>
           <a:ext cx="2009447" cy="605117"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4081,12 +3969,12 @@
       <sheetName val="ML-AN"/>
       <sheetName val="ML-AN-DL"/>
       <sheetName val="ML-F-AI"/>
+      <sheetName val="GH"/>
       <sheetName val="CS"/>
-      <sheetName val="GH"/>
       <sheetName val="FrontEnd"/>
       <sheetName val="Math"/>
+      <sheetName val="Phy"/>
       <sheetName val="Stat"/>
-      <sheetName val="Phy"/>
       <sheetName val="Fin Books"/>
       <sheetName val="BIWS"/>
       <sheetName val="Valuation"/>
@@ -4415,14 +4303,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F4609E-0D16-438A-BB7E-E7C6F41BF509}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736C35BB-D48B-46AE-A0F3-B9591BDF43BE}">
   <sheetPr codeName="Sheet51">
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A2:XFD536"/>
+  <dimension ref="A2:XFD533"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4432,7 +4320,7 @@
     <col min="3" max="3" width="74.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="71.28515625" style="4" customWidth="1"/>
     <col min="5" max="5" width="62.42578125" customWidth="1"/>
-    <col min="6" max="6" width="40.42578125" style="26" customWidth="1"/>
+    <col min="6" max="6" width="40.42578125" style="25" customWidth="1"/>
     <col min="7" max="7" width="27.42578125" customWidth="1"/>
     <col min="8" max="8" width="27.140625" customWidth="1"/>
     <col min="9" max="9" width="42.140625" customWidth="1"/>
@@ -4458,48 +4346,22 @@
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="5"/>
     </row>
     <row r="4" spans="1:12" ht="131.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="D4" s="7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="8"/>
@@ -4507,138 +4369,140 @@
       <c r="H4" s="4"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:12" ht="255" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="9"/>
       <c r="H5" s="4"/>
       <c r="I5" s="10"/>
     </row>
-    <row r="6" spans="1:12" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="255" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="9"/>
       <c r="H6" s="4"/>
       <c r="I6" s="10"/>
     </row>
-    <row r="7" spans="1:12" ht="138" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+    <row r="7" spans="1:12" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>2</v>
+      </c>
       <c r="B7" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F7" s="5"/>
       <c r="G7" s="9"/>
       <c r="H7" s="4"/>
       <c r="I7" s="10"/>
     </row>
-    <row r="8" spans="1:12" ht="240" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>3</v>
-      </c>
+    <row r="8" spans="1:12" ht="138" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E8" s="4"/>
       <c r="F8" s="5"/>
       <c r="G8" s="9"/>
       <c r="H8" s="4"/>
       <c r="I8" s="10"/>
     </row>
-    <row r="9" spans="1:12" ht="242.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="240" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="9"/>
       <c r="H9" s="4"/>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="242.25" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="F10" s="5"/>
       <c r="G10" s="9"/>
       <c r="H10" s="4"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="5"/>
@@ -4646,18 +4510,18 @@
       <c r="H11" s="4"/>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:12" ht="207.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="5"/>
@@ -4665,18 +4529,18 @@
       <c r="H12" s="4"/>
       <c r="I12" s="10"/>
     </row>
-    <row r="13" spans="1:12" ht="197.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="207.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>37</v>
+        <v>32</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="5"/>
@@ -4684,15 +4548,18 @@
       <c r="H13" s="4"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:12" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="197.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="5"/>
@@ -4700,53 +4567,57 @@
       <c r="H14" s="4"/>
       <c r="I14" s="10"/>
     </row>
-    <row r="15" spans="1:12" ht="141" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="9"/>
       <c r="H15" s="4"/>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:12" ht="99.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="D16" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
+    <row r="16" spans="1:12" ht="141" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>10</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="G16" s="9"/>
       <c r="H16" s="4"/>
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:12 16384:16384" ht="167.25" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="5"/>
@@ -4754,120 +4625,100 @@
       <c r="H17" s="4"/>
       <c r="I17" s="10"/>
     </row>
-    <row r="18" spans="1:12 16384:16384" ht="137.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12 16384:16384" ht="165" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="4"/>
       <c r="F18" s="5"/>
       <c r="G18" s="9"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="10"/>
-    </row>
-    <row r="19" spans="1:12 16384:16384" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="1:12 16384:16384" ht="165" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>53</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="5"/>
       <c r="G19" s="9"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="12"/>
-    </row>
-    <row r="20" spans="1:12 16384:16384" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:12 16384:16384" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="5"/>
       <c r="G20" s="9"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:12 16384:16384" ht="165" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>5</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="4" t="s">
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:12 16384:16384" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="9"/>
       <c r="H21" s="4"/>
-      <c r="I21" s="13"/>
-    </row>
-    <row r="22" spans="1:12 16384:16384" ht="165" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>6</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>61</v>
-      </c>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:12 16384:16384" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
       <c r="G22" s="9"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="14"/>
-    </row>
-    <row r="23" spans="1:12 16384:16384" ht="135" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>7</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>64</v>
-      </c>
+    </row>
+    <row r="23" spans="1:12 16384:16384" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
       <c r="E23" s="4"/>
       <c r="F23" s="5"/>
       <c r="G23" s="9"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="1:12 16384:16384" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:12 16384:16384" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="E24" s="4"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="15" t="s">
-        <v>65</v>
-      </c>
+      <c r="G24" s="9"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:12 16384:16384" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
@@ -4876,20 +4727,26 @@
       <c r="F25" s="5"/>
       <c r="G25" s="9"/>
       <c r="H25" s="4"/>
+      <c r="XFD25">
+        <f>SUM(A25:XFC25)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:12 16384:16384" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
+      <c r="B26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="5"/>
       <c r="G26" s="9"/>
       <c r="H26" s="4"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
     </row>
     <row r="27" spans="1:12 16384:16384" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
+      <c r="B27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="5"/>
       <c r="G27" s="9"/>
@@ -4902,10 +4759,6 @@
       <c r="F28" s="5"/>
       <c r="G28" s="9"/>
       <c r="H28" s="4"/>
-      <c r="XFD28">
-        <f>SUM(A28:XFC28)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="29" spans="1:12 16384:16384" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
@@ -4914,10 +4767,6 @@
       <c r="F29" s="5"/>
       <c r="G29" s="9"/>
       <c r="H29" s="4"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
     </row>
     <row r="30" spans="1:12 16384:16384" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
@@ -4960,7 +4809,9 @@
       <c r="H34" s="4"/>
     </row>
     <row r="35" spans="1:8" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
+      <c r="A35" s="4">
+        <v>81</v>
+      </c>
       <c r="B35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="5"/>
@@ -4968,7 +4819,9 @@
       <c r="H35" s="4"/>
     </row>
     <row r="36" spans="1:8" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
+      <c r="A36" s="4">
+        <v>82</v>
+      </c>
       <c r="B36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="5"/>
@@ -4976,7 +4829,9 @@
       <c r="H36" s="4"/>
     </row>
     <row r="37" spans="1:8" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
+      <c r="A37" s="4">
+        <v>83</v>
+      </c>
       <c r="B37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="5"/>
@@ -4985,37 +4840,37 @@
     </row>
     <row r="38" spans="1:8" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B38" s="4"/>
-      <c r="E38" s="4"/>
+      <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="9"/>
       <c r="H38" s="4"/>
     </row>
     <row r="39" spans="1:8" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B39" s="4"/>
-      <c r="E39" s="4"/>
+      <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="9"/>
       <c r="H39" s="4"/>
     </row>
     <row r="40" spans="1:8" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B40" s="4"/>
-      <c r="E40" s="4"/>
+      <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="9"/>
       <c r="H40" s="4"/>
     </row>
     <row r="41" spans="1:8" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B41" s="4"/>
       <c r="E41" s="5"/>
@@ -5025,7 +4880,7 @@
     </row>
     <row r="42" spans="1:8" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B42" s="4"/>
       <c r="E42" s="5"/>
@@ -5035,7 +4890,7 @@
     </row>
     <row r="43" spans="1:8" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B43" s="4"/>
       <c r="E43" s="5"/>
@@ -5045,7 +4900,7 @@
     </row>
     <row r="44" spans="1:8" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B44" s="4"/>
       <c r="E44" s="5"/>
@@ -5055,7 +4910,7 @@
     </row>
     <row r="45" spans="1:8" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B45" s="4"/>
       <c r="E45" s="5"/>
@@ -5065,7 +4920,7 @@
     </row>
     <row r="46" spans="1:8" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B46" s="4"/>
       <c r="E46" s="5"/>
@@ -5075,7 +4930,7 @@
     </row>
     <row r="47" spans="1:8" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B47" s="4"/>
       <c r="E47" s="5"/>
@@ -5085,7 +4940,7 @@
     </row>
     <row r="48" spans="1:8" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B48" s="4"/>
       <c r="E48" s="5"/>
@@ -5093,9 +4948,9 @@
       <c r="G48" s="9"/>
       <c r="H48" s="4"/>
     </row>
-    <row r="49" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B49" s="4"/>
       <c r="E49" s="5"/>
@@ -5103,89 +4958,89 @@
       <c r="G49" s="9"/>
       <c r="H49" s="4"/>
     </row>
-    <row r="50" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
-        <v>93</v>
-      </c>
-      <c r="B50" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="B50" s="15"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
       <c r="G50" s="9"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
-        <v>94</v>
-      </c>
-      <c r="B51" s="4"/>
+        <v>97</v>
+      </c>
+      <c r="B51" s="15"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="4"/>
-    </row>
-    <row r="52" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G51" s="17"/>
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
-        <v>95</v>
-      </c>
-      <c r="B52" s="4"/>
+        <v>98</v>
+      </c>
+      <c r="B52" s="15"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="4"/>
-    </row>
-    <row r="53" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G52" s="17"/>
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
-        <v>96</v>
-      </c>
-      <c r="B53" s="16"/>
+        <v>99</v>
+      </c>
+      <c r="B53" s="15"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="4"/>
-    </row>
-    <row r="54" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G53" s="17"/>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
-        <v>97</v>
-      </c>
-      <c r="B54" s="16"/>
+        <v>100</v>
+      </c>
+      <c r="B54" s="4"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
-      <c r="G54" s="18"/>
-      <c r="H54" s="5"/>
-    </row>
-    <row r="55" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G54" s="9"/>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
-        <v>98</v>
-      </c>
-      <c r="B55" s="16"/>
-      <c r="E55" s="5"/>
+        <v>101</v>
+      </c>
+      <c r="B55" s="4"/>
+      <c r="E55" s="4"/>
       <c r="F55" s="5"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="5"/>
-    </row>
-    <row r="56" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G55" s="9"/>
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
-        <v>99</v>
-      </c>
-      <c r="B56" s="16"/>
-      <c r="E56" s="5"/>
+        <v>102</v>
+      </c>
+      <c r="B56" s="4"/>
+      <c r="E56" s="4"/>
       <c r="F56" s="5"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="5"/>
-    </row>
-    <row r="57" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G56" s="9"/>
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B57" s="4"/>
-      <c r="E57" s="5"/>
+      <c r="E57" s="4"/>
       <c r="F57" s="5"/>
       <c r="G57" s="9"/>
       <c r="H57" s="4"/>
     </row>
-    <row r="58" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B58" s="4"/>
       <c r="E58" s="4"/>
@@ -5193,9 +5048,9 @@
       <c r="G58" s="9"/>
       <c r="H58" s="4"/>
     </row>
-    <row r="59" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B59" s="4"/>
       <c r="E59" s="4"/>
@@ -5203,9 +5058,9 @@
       <c r="G59" s="9"/>
       <c r="H59" s="4"/>
     </row>
-    <row r="60" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B60" s="4"/>
       <c r="E60" s="4"/>
@@ -5213,39 +5068,46 @@
       <c r="G60" s="9"/>
       <c r="H60" s="4"/>
     </row>
-    <row r="61" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B61" s="4"/>
       <c r="E61" s="4"/>
       <c r="F61" s="5"/>
       <c r="G61" s="9"/>
       <c r="H61" s="4"/>
-    </row>
-    <row r="62" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+    </row>
+    <row r="62" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B62" s="4"/>
       <c r="E62" s="4"/>
       <c r="F62" s="5"/>
       <c r="G62" s="9"/>
       <c r="H62" s="4"/>
-    </row>
-    <row r="63" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+    </row>
+    <row r="63" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B63" s="4"/>
       <c r="E63" s="4"/>
       <c r="F63" s="5"/>
       <c r="G63" s="9"/>
       <c r="H63" s="4"/>
-    </row>
-    <row r="64" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="4"/>
+    </row>
+    <row r="64" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B64" s="4"/>
       <c r="E64" s="4"/>
@@ -5253,11 +5115,10 @@
       <c r="G64" s="9"/>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-    </row>
-    <row r="65" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:9" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B65" s="4"/>
       <c r="E65" s="4"/>
@@ -5265,11 +5126,10 @@
       <c r="G65" s="9"/>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
-    </row>
-    <row r="66" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:9" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B66" s="4"/>
       <c r="E66" s="4"/>
@@ -5277,12 +5137,10 @@
       <c r="G66" s="9"/>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-    </row>
-    <row r="67" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:9" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B67" s="4"/>
       <c r="E67" s="4"/>
@@ -5291,9 +5149,9 @@
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
     </row>
-    <row r="68" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B68" s="4"/>
       <c r="E68" s="4"/>
@@ -5302,42 +5160,42 @@
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
     </row>
-    <row r="69" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B69" s="4"/>
       <c r="E69" s="4"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="9"/>
+      <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
     </row>
-    <row r="70" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B70" s="4"/>
       <c r="E70" s="4"/>
       <c r="F70" s="5"/>
-      <c r="G70" s="9"/>
+      <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
     </row>
-    <row r="71" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B71" s="4"/>
       <c r="E71" s="4"/>
       <c r="F71" s="5"/>
-      <c r="G71" s="9"/>
+      <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
     </row>
-    <row r="72" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B72" s="4"/>
       <c r="E72" s="4"/>
@@ -5346,9 +5204,9 @@
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
     </row>
-    <row r="73" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B73" s="4"/>
       <c r="E73" s="4"/>
@@ -5357,9 +5215,9 @@
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
     </row>
-    <row r="74" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B74" s="4"/>
       <c r="E74" s="4"/>
@@ -5368,9 +5226,9 @@
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
     </row>
-    <row r="75" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B75" s="4"/>
       <c r="E75" s="4"/>
@@ -5379,9 +5237,9 @@
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
     </row>
-    <row r="76" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B76" s="4"/>
       <c r="E76" s="4"/>
@@ -5390,9 +5248,9 @@
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
     </row>
-    <row r="77" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B77" s="4"/>
       <c r="E77" s="4"/>
@@ -5401,9 +5259,9 @@
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
     </row>
-    <row r="78" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B78" s="4"/>
       <c r="E78" s="4"/>
@@ -5412,9 +5270,9 @@
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B79" s="4"/>
       <c r="E79" s="4"/>
@@ -5423,9 +5281,9 @@
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B80" s="4"/>
       <c r="E80" s="4"/>
@@ -5434,42 +5292,39 @@
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B81" s="4"/>
       <c r="E81" s="4"/>
       <c r="F81" s="5"/>
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
-      <c r="I81" s="4"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B82" s="4"/>
       <c r="E82" s="4"/>
       <c r="F82" s="5"/>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
-      <c r="I82" s="4"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B83" s="4"/>
       <c r="E83" s="4"/>
       <c r="F83" s="5"/>
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
-      <c r="I83" s="4"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B84" s="4"/>
       <c r="E84" s="4"/>
@@ -5477,39 +5332,42 @@
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B85" s="4"/>
+      <c r="D85"/>
       <c r="E85" s="4"/>
       <c r="F85" s="5"/>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B86" s="4"/>
+      <c r="D86"/>
       <c r="E86" s="4"/>
       <c r="F86" s="5"/>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B87" s="4"/>
+      <c r="D87"/>
       <c r="E87" s="4"/>
       <c r="F87" s="5"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B88" s="4"/>
       <c r="D88"/>
@@ -5518,9 +5376,9 @@
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B89" s="4"/>
       <c r="D89"/>
@@ -5529,9 +5387,9 @@
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B90" s="4"/>
       <c r="D90"/>
@@ -5540,9 +5398,9 @@
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B91" s="4"/>
       <c r="D91"/>
@@ -5551,42 +5409,39 @@
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B92" s="4"/>
-      <c r="D92"/>
       <c r="E92" s="4"/>
       <c r="F92" s="5"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B93" s="4"/>
-      <c r="D93"/>
       <c r="E93" s="4"/>
       <c r="F93" s="5"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B94" s="4"/>
-      <c r="D94"/>
       <c r="E94" s="4"/>
       <c r="F94" s="5"/>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B95" s="4"/>
       <c r="E95" s="4"/>
@@ -5594,9 +5449,9 @@
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B96" s="4"/>
       <c r="E96" s="4"/>
@@ -5606,7 +5461,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B97" s="4"/>
       <c r="E97" s="4"/>
@@ -5616,7 +5471,7 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B98" s="4"/>
       <c r="E98" s="4"/>
@@ -5626,7 +5481,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B99" s="4"/>
       <c r="E99" s="4"/>
@@ -5636,7 +5491,7 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B100" s="4"/>
       <c r="E100" s="4"/>
@@ -5646,7 +5501,7 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B101" s="4"/>
       <c r="E101" s="4"/>
@@ -5656,9 +5511,9 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
-        <v>145</v>
-      </c>
-      <c r="B102" s="4"/>
+        <v>148</v>
+      </c>
+      <c r="B102" s="18"/>
       <c r="E102" s="4"/>
       <c r="F102" s="5"/>
       <c r="G102" s="4"/>
@@ -5666,9 +5521,10 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
-        <v>146</v>
-      </c>
-      <c r="B103" s="4"/>
+        <v>149</v>
+      </c>
+      <c r="B103" s="19"/>
+      <c r="C103" s="20"/>
       <c r="E103" s="4"/>
       <c r="F103" s="5"/>
       <c r="G103" s="4"/>
@@ -5676,7 +5532,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B104" s="4"/>
       <c r="E104" s="4"/>
@@ -5686,9 +5542,9 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
-        <v>148</v>
-      </c>
-      <c r="B105" s="19"/>
+        <v>151</v>
+      </c>
+      <c r="B105" s="4"/>
       <c r="E105" s="4"/>
       <c r="F105" s="5"/>
       <c r="G105" s="4"/>
@@ -5696,10 +5552,9 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
-        <v>149</v>
-      </c>
-      <c r="B106" s="20"/>
-      <c r="C106" s="21"/>
+        <v>152</v>
+      </c>
+      <c r="B106" s="4"/>
       <c r="E106" s="4"/>
       <c r="F106" s="5"/>
       <c r="G106" s="4"/>
@@ -5707,7 +5562,7 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B107" s="4"/>
       <c r="E107" s="4"/>
@@ -5717,7 +5572,7 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B108" s="4"/>
       <c r="E108" s="4"/>
@@ -5727,7 +5582,7 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B109" s="4"/>
       <c r="E109" s="4"/>
@@ -5737,7 +5592,7 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B110" s="4"/>
       <c r="E110" s="4"/>
@@ -5745,9 +5600,9 @@
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B111" s="4"/>
       <c r="E111" s="4"/>
@@ -5757,7 +5612,7 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B112" s="4"/>
       <c r="E112" s="4"/>
@@ -5767,7 +5622,7 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B113" s="4"/>
       <c r="E113" s="4"/>
@@ -5775,9 +5630,9 @@
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
     </row>
-    <row r="114" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B114" s="4"/>
       <c r="E114" s="4"/>
@@ -5787,7 +5642,7 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B115" s="4"/>
       <c r="E115" s="4"/>
@@ -5797,7 +5652,7 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B116" s="4"/>
       <c r="E116" s="4"/>
@@ -5807,7 +5662,7 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B117" s="4"/>
       <c r="E117" s="4"/>
@@ -5817,7 +5672,7 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B118" s="4"/>
       <c r="E118" s="4"/>
@@ -5827,7 +5682,7 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B119" s="4"/>
       <c r="E119" s="4"/>
@@ -5837,7 +5692,7 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B120" s="4"/>
       <c r="E120" s="4"/>
@@ -5847,7 +5702,7 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B121" s="4"/>
       <c r="E121" s="4"/>
@@ -5857,7 +5712,7 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B122" s="4"/>
       <c r="E122" s="4"/>
@@ -5867,7 +5722,7 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B123" s="4"/>
       <c r="E123" s="4"/>
@@ -5877,7 +5732,7 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B124" s="4"/>
       <c r="E124" s="4"/>
@@ -5887,7 +5742,7 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B125" s="4"/>
       <c r="E125" s="4"/>
@@ -5897,7 +5752,7 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B126" s="4"/>
       <c r="E126" s="4"/>
@@ -5907,7 +5762,7 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B127" s="4"/>
       <c r="E127" s="4"/>
@@ -5917,7 +5772,7 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B128" s="4"/>
       <c r="E128" s="4"/>
@@ -5927,7 +5782,7 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B129" s="4"/>
       <c r="E129" s="4"/>
@@ -5937,7 +5792,7 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B130" s="4"/>
       <c r="E130" s="4"/>
@@ -5947,7 +5802,7 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B131" s="4"/>
       <c r="E131" s="4"/>
@@ -5957,7 +5812,7 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B132" s="4"/>
       <c r="E132" s="4"/>
@@ -5967,7 +5822,7 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="4">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B133" s="4"/>
       <c r="E133" s="4"/>
@@ -5977,7 +5832,7 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B134" s="4"/>
       <c r="E134" s="4"/>
@@ -5987,7 +5842,7 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B135" s="4"/>
       <c r="E135" s="4"/>
@@ -5995,353 +5850,356 @@
       <c r="G135" s="4"/>
       <c r="H135" s="4"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
-        <v>179</v>
-      </c>
-      <c r="B136" s="4"/>
-      <c r="E136" s="4"/>
-      <c r="F136" s="5"/>
-      <c r="G136" s="4"/>
-      <c r="H136" s="4"/>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="B136" s="18"/>
+      <c r="C136" s="18"/>
+      <c r="D136" s="18"/>
+      <c r="E136" s="18"/>
+      <c r="F136" s="21"/>
+      <c r="G136" s="22"/>
+      <c r="H136" s="22"/>
+    </row>
+    <row r="137" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
-        <v>180</v>
-      </c>
-      <c r="B137" s="4"/>
-      <c r="E137" s="4"/>
-      <c r="F137" s="5"/>
-      <c r="G137" s="4"/>
-      <c r="H137" s="4"/>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="B137" s="18"/>
+      <c r="C137" s="18"/>
+      <c r="D137" s="18"/>
+      <c r="E137" s="18"/>
+      <c r="F137" s="21"/>
+      <c r="G137" s="22"/>
+      <c r="H137" s="22"/>
+    </row>
+    <row r="138" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
-        <v>181</v>
-      </c>
-      <c r="B138" s="4"/>
-      <c r="E138" s="4"/>
-      <c r="F138" s="5"/>
-      <c r="G138" s="4"/>
-      <c r="H138" s="4"/>
-    </row>
-    <row r="139" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="B138" s="18"/>
+      <c r="C138" s="18"/>
+      <c r="D138" s="18"/>
+      <c r="E138" s="18"/>
+      <c r="F138" s="21"/>
+      <c r="G138" s="22"/>
+      <c r="H138" s="22"/>
+    </row>
+    <row r="139" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
-        <v>182</v>
-      </c>
-      <c r="B139" s="19"/>
-      <c r="C139" s="19"/>
-      <c r="D139" s="19"/>
-      <c r="E139" s="19"/>
-      <c r="F139" s="22"/>
-      <c r="G139" s="23"/>
-      <c r="H139" s="23"/>
-    </row>
-    <row r="140" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+      <c r="B139" s="18"/>
+      <c r="C139" s="18"/>
+      <c r="D139" s="18"/>
+      <c r="E139" s="18"/>
+      <c r="F139" s="21"/>
+      <c r="G139" s="22"/>
+      <c r="H139" s="22"/>
+    </row>
+    <row r="140" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
-        <v>183</v>
-      </c>
-      <c r="B140" s="19"/>
-      <c r="C140" s="19"/>
-      <c r="D140" s="19"/>
-      <c r="E140" s="19"/>
-      <c r="F140" s="22"/>
-      <c r="G140" s="23"/>
-      <c r="H140" s="23"/>
-    </row>
-    <row r="141" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="B140" s="18"/>
+      <c r="C140" s="18"/>
+      <c r="D140" s="18"/>
+      <c r="E140" s="18"/>
+      <c r="F140" s="21"/>
+      <c r="G140" s="22"/>
+      <c r="H140" s="22"/>
+    </row>
+    <row r="141" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
-        <v>184</v>
-      </c>
-      <c r="B141" s="19"/>
-      <c r="C141" s="19"/>
-      <c r="D141" s="19"/>
-      <c r="E141" s="19"/>
-      <c r="F141" s="22"/>
-      <c r="G141" s="23"/>
-      <c r="H141" s="23"/>
-    </row>
-    <row r="142" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="B141" s="18"/>
+      <c r="C141" s="18"/>
+      <c r="D141" s="18"/>
+      <c r="E141" s="18"/>
+      <c r="F141" s="21"/>
+      <c r="G141" s="22"/>
+      <c r="H141" s="22"/>
+    </row>
+    <row r="142" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
-        <v>185</v>
-      </c>
-      <c r="B142" s="19"/>
-      <c r="C142" s="19"/>
-      <c r="D142" s="19"/>
-      <c r="E142" s="19"/>
-      <c r="F142" s="22"/>
-      <c r="G142" s="23"/>
-      <c r="H142" s="23"/>
-    </row>
-    <row r="143" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="B142" s="18"/>
+      <c r="C142" s="18"/>
+      <c r="D142" s="18"/>
+      <c r="E142" s="18"/>
+      <c r="F142" s="21"/>
+      <c r="G142" s="22"/>
+      <c r="H142" s="22"/>
+    </row>
+    <row r="143" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
-        <v>186</v>
-      </c>
-      <c r="B143" s="19"/>
-      <c r="C143" s="19"/>
-      <c r="D143" s="19"/>
-      <c r="E143" s="19"/>
-      <c r="F143" s="22"/>
-      <c r="G143" s="23"/>
-      <c r="H143" s="23"/>
-    </row>
-    <row r="144" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="B143" s="18"/>
+      <c r="C143" s="18"/>
+      <c r="D143" s="18"/>
+      <c r="E143" s="18"/>
+      <c r="F143" s="21"/>
+      <c r="G143" s="22"/>
+      <c r="H143" s="22"/>
+    </row>
+    <row r="144" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
-        <v>187</v>
-      </c>
-      <c r="B144" s="19"/>
-      <c r="C144" s="19"/>
-      <c r="D144" s="19"/>
-      <c r="E144" s="19"/>
-      <c r="F144" s="22"/>
-      <c r="G144" s="23"/>
-      <c r="H144" s="23"/>
-    </row>
-    <row r="145" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+      <c r="B144" s="18"/>
+      <c r="C144" s="18"/>
+      <c r="D144" s="18"/>
+      <c r="E144" s="18"/>
+      <c r="F144" s="21"/>
+      <c r="G144" s="22"/>
+      <c r="H144" s="22"/>
+    </row>
+    <row r="145" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="4">
-        <v>188</v>
-      </c>
-      <c r="B145" s="19"/>
-      <c r="C145" s="19"/>
-      <c r="D145" s="19"/>
-      <c r="E145" s="19"/>
-      <c r="F145" s="22"/>
-      <c r="G145" s="23"/>
-      <c r="H145" s="23"/>
-    </row>
-    <row r="146" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="B145" s="18"/>
+      <c r="C145" s="18"/>
+      <c r="D145" s="18"/>
+      <c r="E145" s="18"/>
+      <c r="F145" s="21"/>
+      <c r="G145" s="22"/>
+      <c r="H145" s="22"/>
+    </row>
+    <row r="146" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
-        <v>189</v>
-      </c>
-      <c r="B146" s="19"/>
-      <c r="C146" s="19"/>
-      <c r="D146" s="19"/>
-      <c r="E146" s="19"/>
-      <c r="F146" s="22"/>
-      <c r="G146" s="23"/>
-      <c r="H146" s="23"/>
-    </row>
-    <row r="147" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+      <c r="B146" s="18"/>
+      <c r="C146" s="18"/>
+      <c r="D146" s="18"/>
+      <c r="E146" s="18"/>
+      <c r="F146" s="21"/>
+      <c r="G146" s="22"/>
+      <c r="H146" s="22"/>
+    </row>
+    <row r="147" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
-        <v>190</v>
-      </c>
-      <c r="B147" s="19"/>
-      <c r="C147" s="19"/>
-      <c r="D147" s="19"/>
-      <c r="E147" s="19"/>
-      <c r="F147" s="22"/>
-      <c r="G147" s="23"/>
-      <c r="H147" s="23"/>
-    </row>
-    <row r="148" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+      <c r="B147" s="18"/>
+      <c r="C147" s="18"/>
+      <c r="D147" s="18"/>
+      <c r="E147" s="18"/>
+      <c r="F147" s="21"/>
+      <c r="G147" s="22"/>
+      <c r="H147" s="22"/>
+    </row>
+    <row r="148" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
-        <v>191</v>
-      </c>
-      <c r="B148" s="19"/>
-      <c r="C148" s="19"/>
-      <c r="D148" s="19"/>
-      <c r="E148" s="19"/>
-      <c r="F148" s="22"/>
-      <c r="G148" s="23"/>
-      <c r="H148" s="23"/>
-    </row>
-    <row r="149" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+      <c r="B148" s="18"/>
+      <c r="C148" s="18"/>
+      <c r="D148" s="18"/>
+      <c r="E148" s="18"/>
+      <c r="F148" s="21"/>
+      <c r="G148" s="22"/>
+      <c r="H148" s="22"/>
+    </row>
+    <row r="149" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
-        <v>192</v>
-      </c>
-      <c r="B149" s="19"/>
-      <c r="C149" s="19"/>
-      <c r="D149" s="19"/>
-      <c r="E149" s="19"/>
-      <c r="F149" s="22"/>
-      <c r="G149" s="23"/>
-      <c r="H149" s="23"/>
-    </row>
-    <row r="150" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+      <c r="B149" s="18"/>
+      <c r="C149" s="18"/>
+      <c r="D149" s="18"/>
+      <c r="E149" s="18"/>
+      <c r="F149" s="21"/>
+      <c r="G149" s="22"/>
+      <c r="H149" s="22"/>
+    </row>
+    <row r="150" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
-        <v>193</v>
-      </c>
-      <c r="B150" s="19"/>
-      <c r="C150" s="19"/>
-      <c r="D150" s="19"/>
-      <c r="E150" s="19"/>
-      <c r="F150" s="22"/>
-      <c r="G150" s="23"/>
-      <c r="H150" s="23"/>
-    </row>
-    <row r="151" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="B150" s="18"/>
+      <c r="C150" s="18"/>
+      <c r="D150" s="18"/>
+      <c r="E150" s="18"/>
+      <c r="F150" s="21"/>
+      <c r="G150" s="22"/>
+      <c r="H150" s="22"/>
+    </row>
+    <row r="151" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="4">
-        <v>194</v>
-      </c>
-      <c r="B151" s="19"/>
-      <c r="C151" s="19"/>
-      <c r="D151" s="19"/>
-      <c r="E151" s="19"/>
-      <c r="F151" s="22"/>
-      <c r="G151" s="23"/>
-      <c r="H151" s="23"/>
-    </row>
-    <row r="152" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+      <c r="B151" s="18"/>
+      <c r="C151" s="18"/>
+      <c r="D151" s="18"/>
+      <c r="E151" s="18"/>
+      <c r="F151" s="21"/>
+      <c r="G151" s="22"/>
+      <c r="H151" s="22"/>
+    </row>
+    <row r="152" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
-        <v>195</v>
-      </c>
-      <c r="B152" s="19"/>
-      <c r="C152" s="19"/>
-      <c r="D152" s="19"/>
-      <c r="E152" s="19"/>
-      <c r="F152" s="22"/>
-      <c r="G152" s="23"/>
-      <c r="H152" s="23"/>
-    </row>
-    <row r="153" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="B152" s="18"/>
+      <c r="C152" s="18"/>
+      <c r="D152" s="18"/>
+      <c r="E152" s="18"/>
+      <c r="F152" s="21"/>
+      <c r="G152" s="22"/>
+      <c r="H152" s="22"/>
+    </row>
+    <row r="153" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="4">
-        <v>196</v>
-      </c>
-      <c r="B153" s="19"/>
-      <c r="C153" s="19"/>
-      <c r="D153" s="19"/>
-      <c r="E153" s="19"/>
-      <c r="F153" s="22"/>
-      <c r="G153" s="23"/>
-      <c r="H153" s="23"/>
-    </row>
-    <row r="154" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="B153" s="18"/>
+      <c r="C153" s="18"/>
+      <c r="D153" s="18"/>
+      <c r="E153" s="18"/>
+      <c r="F153" s="21"/>
+      <c r="G153" s="22"/>
+      <c r="H153" s="22"/>
+    </row>
+    <row r="154" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="4">
-        <v>197</v>
-      </c>
-      <c r="B154" s="19"/>
-      <c r="C154" s="19"/>
-      <c r="D154" s="19"/>
-      <c r="E154" s="19"/>
-      <c r="F154" s="22"/>
-      <c r="G154" s="23"/>
-      <c r="H154" s="23"/>
-    </row>
-    <row r="155" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="B154" s="18"/>
+      <c r="C154" s="18"/>
+      <c r="D154" s="18"/>
+      <c r="E154" s="18"/>
+      <c r="F154" s="21"/>
+      <c r="G154" s="22"/>
+      <c r="H154" s="22"/>
+    </row>
+    <row r="155" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="4">
-        <v>198</v>
-      </c>
-      <c r="B155" s="19"/>
-      <c r="C155" s="19"/>
-      <c r="D155" s="19"/>
-      <c r="E155" s="19"/>
-      <c r="F155" s="22"/>
-      <c r="G155" s="23"/>
-      <c r="H155" s="23"/>
-    </row>
-    <row r="156" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+      <c r="B155" s="18"/>
+      <c r="C155" s="24"/>
+      <c r="D155" s="18"/>
+      <c r="E155" s="18"/>
+      <c r="F155" s="21"/>
+      <c r="G155" s="22"/>
+      <c r="H155" s="22"/>
+    </row>
+    <row r="156" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="4">
-        <v>199</v>
-      </c>
-      <c r="B156" s="19"/>
-      <c r="C156" s="19"/>
-      <c r="D156" s="19"/>
-      <c r="E156" s="19"/>
-      <c r="F156" s="22"/>
-      <c r="G156" s="23"/>
-      <c r="H156" s="23"/>
-    </row>
-    <row r="157" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="B156" s="18"/>
+      <c r="C156" s="18"/>
+      <c r="D156" s="18"/>
+      <c r="E156" s="18"/>
+      <c r="F156" s="21"/>
+      <c r="G156" s="22"/>
+      <c r="H156" s="22"/>
+    </row>
+    <row r="157" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="4">
-        <v>200</v>
-      </c>
-      <c r="B157" s="19"/>
-      <c r="C157" s="19"/>
-      <c r="D157" s="19"/>
-      <c r="E157" s="19"/>
-      <c r="F157" s="22"/>
-      <c r="G157" s="23"/>
-      <c r="H157" s="23"/>
-    </row>
-    <row r="158" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+      <c r="B157" s="18"/>
+      <c r="C157" s="18"/>
+      <c r="D157" s="18"/>
+      <c r="E157" s="18"/>
+      <c r="F157" s="21"/>
+      <c r="G157" s="22"/>
+      <c r="H157" s="22"/>
+    </row>
+    <row r="158" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="4">
-        <v>201</v>
-      </c>
-      <c r="B158" s="19"/>
-      <c r="C158" s="25"/>
-      <c r="D158" s="19"/>
-      <c r="E158" s="19"/>
-      <c r="F158" s="22"/>
-      <c r="G158" s="23"/>
-      <c r="H158" s="23"/>
-    </row>
-    <row r="159" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="B158" s="18"/>
+      <c r="C158" s="18"/>
+      <c r="D158" s="18"/>
+      <c r="E158" s="18"/>
+      <c r="F158" s="21"/>
+      <c r="G158" s="22"/>
+      <c r="H158" s="22"/>
+    </row>
+    <row r="159" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="4">
-        <v>202</v>
-      </c>
-      <c r="B159" s="19"/>
-      <c r="C159" s="19"/>
-      <c r="D159" s="19"/>
-      <c r="E159" s="19"/>
-      <c r="F159" s="22"/>
-      <c r="G159" s="23"/>
-      <c r="H159" s="23"/>
-    </row>
-    <row r="160" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="B159" s="18"/>
+      <c r="C159" s="18"/>
+      <c r="D159" s="18"/>
+      <c r="E159" s="18"/>
+      <c r="F159" s="21"/>
+      <c r="G159" s="22"/>
+      <c r="H159" s="22"/>
+    </row>
+    <row r="160" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="4">
-        <v>203</v>
-      </c>
-      <c r="B160" s="19"/>
-      <c r="C160" s="19"/>
-      <c r="D160" s="19"/>
-      <c r="E160" s="19"/>
-      <c r="F160" s="22"/>
-      <c r="G160" s="23"/>
-      <c r="H160" s="23"/>
-    </row>
-    <row r="161" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="B160" s="18"/>
+      <c r="C160" s="24"/>
+      <c r="D160" s="18"/>
+      <c r="E160" s="18"/>
+      <c r="F160" s="21"/>
+      <c r="G160" s="22"/>
+      <c r="H160" s="22"/>
+    </row>
+    <row r="161" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
-        <v>204</v>
-      </c>
-      <c r="B161" s="19"/>
-      <c r="C161" s="19"/>
-      <c r="D161" s="19"/>
-      <c r="E161" s="19"/>
-      <c r="F161" s="22"/>
-      <c r="G161" s="23"/>
-      <c r="H161" s="23"/>
-    </row>
-    <row r="162" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="B161" s="18"/>
+      <c r="C161" s="18"/>
+      <c r="D161" s="18"/>
+      <c r="E161" s="18"/>
+      <c r="F161" s="21"/>
+      <c r="G161" s="22"/>
+      <c r="H161" s="22"/>
+    </row>
+    <row r="162" spans="1:8" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="4">
-        <v>205</v>
-      </c>
-      <c r="B162" s="19"/>
-      <c r="C162" s="19"/>
-      <c r="D162" s="19"/>
-      <c r="E162" s="19"/>
-      <c r="F162" s="22"/>
-      <c r="G162" s="23"/>
-      <c r="H162" s="23"/>
-    </row>
-    <row r="163" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="B162" s="4"/>
+      <c r="E162" s="4"/>
+      <c r="F162" s="5"/>
+      <c r="G162" s="4"/>
+      <c r="H162" s="4"/>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="4">
-        <v>206</v>
-      </c>
-      <c r="B163" s="19"/>
-      <c r="C163" s="25"/>
-      <c r="D163" s="19"/>
-      <c r="E163" s="19"/>
-      <c r="F163" s="22"/>
-      <c r="G163" s="23"/>
-      <c r="H163" s="23"/>
-    </row>
-    <row r="164" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+      <c r="B163" s="4"/>
+      <c r="C163" s="11"/>
+      <c r="E163" s="4"/>
+      <c r="F163" s="5"/>
+      <c r="G163" s="4"/>
+      <c r="H163" s="4"/>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="4">
-        <v>207</v>
-      </c>
-      <c r="B164" s="19"/>
-      <c r="C164" s="19"/>
-      <c r="D164" s="19"/>
-      <c r="E164" s="19"/>
-      <c r="F164" s="22"/>
-      <c r="G164" s="23"/>
-      <c r="H164" s="23"/>
-    </row>
-    <row r="165" spans="1:8" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="B164" s="4"/>
+      <c r="C164" s="11"/>
+      <c r="E164" s="4"/>
+      <c r="F164" s="5"/>
+      <c r="G164" s="4"/>
+      <c r="H164" s="4"/>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="4">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B165" s="4"/>
+      <c r="C165" s="11"/>
       <c r="E165" s="4"/>
       <c r="F165" s="5"/>
       <c r="G165" s="4"/>
@@ -6349,10 +6207,9 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="4">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B166" s="4"/>
-      <c r="C166" s="11"/>
       <c r="E166" s="4"/>
       <c r="F166" s="5"/>
       <c r="G166" s="4"/>
@@ -6360,10 +6217,9 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="4">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B167" s="4"/>
-      <c r="C167" s="11"/>
       <c r="E167" s="4"/>
       <c r="F167" s="5"/>
       <c r="G167" s="4"/>
@@ -6371,7 +6227,7 @@
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="4">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B168" s="4"/>
       <c r="C168" s="11"/>
@@ -6382,7 +6238,7 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="4">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B169" s="4"/>
       <c r="E169" s="4"/>
@@ -6392,7 +6248,7 @@
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="4">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B170" s="4"/>
       <c r="E170" s="4"/>
@@ -6402,10 +6258,9 @@
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="4">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B171" s="4"/>
-      <c r="C171" s="11"/>
       <c r="E171" s="4"/>
       <c r="F171" s="5"/>
       <c r="G171" s="4"/>
@@ -6413,9 +6268,10 @@
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="4">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B172" s="4"/>
+      <c r="C172" s="11"/>
       <c r="E172" s="4"/>
       <c r="F172" s="5"/>
       <c r="G172" s="4"/>
@@ -6423,19 +6279,21 @@
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="4">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B173" s="4"/>
+      <c r="C173" s="11"/>
       <c r="E173" s="4"/>
       <c r="F173" s="5"/>
       <c r="G173" s="4"/>
       <c r="H173" s="4"/>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="4">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B174" s="4"/>
+      <c r="C174" s="11"/>
       <c r="E174" s="4"/>
       <c r="F174" s="5"/>
       <c r="G174" s="4"/>
@@ -6443,7 +6301,7 @@
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="4">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B175" s="4"/>
       <c r="C175" s="11"/>
@@ -6454,7 +6312,7 @@
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="4">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B176" s="4"/>
       <c r="C176" s="11"/>
@@ -6463,9 +6321,9 @@
       <c r="G176" s="4"/>
       <c r="H176" s="4"/>
     </row>
-    <row r="177" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="4">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B177" s="4"/>
       <c r="C177" s="11"/>
@@ -6476,7 +6334,7 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="4">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B178" s="4"/>
       <c r="C178" s="11"/>
@@ -6487,7 +6345,7 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="4">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B179" s="4"/>
       <c r="C179" s="11"/>
@@ -6498,7 +6356,7 @@
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="4">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B180" s="4"/>
       <c r="C180" s="11"/>
@@ -6509,10 +6367,9 @@
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="4">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B181" s="4"/>
-      <c r="C181" s="11"/>
       <c r="E181" s="4"/>
       <c r="F181" s="5"/>
       <c r="G181" s="4"/>
@@ -6520,10 +6377,9 @@
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="4">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B182" s="4"/>
-      <c r="C182" s="11"/>
       <c r="E182" s="4"/>
       <c r="F182" s="5"/>
       <c r="G182" s="4"/>
@@ -6531,10 +6387,9 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="4">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B183" s="4"/>
-      <c r="C183" s="11"/>
       <c r="E183" s="4"/>
       <c r="F183" s="5"/>
       <c r="G183" s="4"/>
@@ -6542,7 +6397,7 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="4">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B184" s="4"/>
       <c r="E184" s="4"/>
@@ -6552,7 +6407,7 @@
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="4">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B185" s="4"/>
       <c r="E185" s="4"/>
@@ -6562,7 +6417,7 @@
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="4">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B186" s="4"/>
       <c r="E186" s="4"/>
@@ -6572,7 +6427,7 @@
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="4">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B187" s="4"/>
       <c r="E187" s="4"/>
@@ -6580,9 +6435,9 @@
       <c r="G187" s="4"/>
       <c r="H187" s="4"/>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="4">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B188" s="4"/>
       <c r="E188" s="4"/>
@@ -6590,9 +6445,9 @@
       <c r="G188" s="4"/>
       <c r="H188" s="4"/>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="4">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B189" s="4"/>
       <c r="E189" s="4"/>
@@ -6600,9 +6455,9 @@
       <c r="G189" s="4"/>
       <c r="H189" s="4"/>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="4">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B190" s="4"/>
       <c r="E190" s="4"/>
@@ -6610,9 +6465,9 @@
       <c r="G190" s="4"/>
       <c r="H190" s="4"/>
     </row>
-    <row r="191" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="4">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B191" s="4"/>
       <c r="E191" s="4"/>
@@ -6620,21 +6475,23 @@
       <c r="G191" s="4"/>
       <c r="H191" s="4"/>
     </row>
-    <row r="192" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="4">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B192" s="4"/>
+      <c r="C192" s="11"/>
       <c r="E192" s="4"/>
       <c r="F192" s="5"/>
       <c r="G192" s="4"/>
       <c r="H192" s="4"/>
     </row>
-    <row r="193" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="4">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B193" s="4"/>
+      <c r="C193" s="11"/>
       <c r="E193" s="4"/>
       <c r="F193" s="5"/>
       <c r="G193" s="4"/>
@@ -6642,9 +6499,10 @@
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="4">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B194" s="4"/>
+      <c r="C194" s="11"/>
       <c r="E194" s="4"/>
       <c r="F194" s="5"/>
       <c r="G194" s="4"/>
@@ -6652,10 +6510,9 @@
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="4">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B195" s="4"/>
-      <c r="C195" s="11"/>
       <c r="E195" s="4"/>
       <c r="F195" s="5"/>
       <c r="G195" s="4"/>
@@ -6663,7 +6520,7 @@
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="4">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B196" s="4"/>
       <c r="C196" s="11"/>
@@ -6672,12 +6529,11 @@
       <c r="G196" s="4"/>
       <c r="H196" s="4"/>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="4">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B197" s="4"/>
-      <c r="C197" s="11"/>
       <c r="E197" s="4"/>
       <c r="F197" s="5"/>
       <c r="G197" s="4"/>
@@ -6685,7 +6541,7 @@
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="4">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B198" s="4"/>
       <c r="E198" s="4"/>
@@ -6695,7 +6551,7 @@
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="4">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B199" s="4"/>
       <c r="C199" s="11"/>
@@ -6704,11 +6560,12 @@
       <c r="G199" s="4"/>
       <c r="H199" s="4"/>
     </row>
-    <row r="200" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="4">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B200" s="4"/>
+      <c r="C200" s="11"/>
       <c r="E200" s="4"/>
       <c r="F200" s="5"/>
       <c r="G200" s="4"/>
@@ -6716,7 +6573,7 @@
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="4">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B201" s="4"/>
       <c r="E201" s="4"/>
@@ -6726,10 +6583,9 @@
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="4">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B202" s="4"/>
-      <c r="C202" s="11"/>
       <c r="E202" s="4"/>
       <c r="F202" s="5"/>
       <c r="G202" s="4"/>
@@ -6737,10 +6593,9 @@
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="4">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B203" s="4"/>
-      <c r="C203" s="11"/>
       <c r="E203" s="4"/>
       <c r="F203" s="5"/>
       <c r="G203" s="4"/>
@@ -6748,7 +6603,7 @@
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="4">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B204" s="4"/>
       <c r="E204" s="4"/>
@@ -6758,9 +6613,10 @@
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="4">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B205" s="4"/>
+      <c r="C205" s="11"/>
       <c r="E205" s="4"/>
       <c r="F205" s="5"/>
       <c r="G205" s="4"/>
@@ -6768,9 +6624,10 @@
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="4">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B206" s="4"/>
+      <c r="C206" s="11"/>
       <c r="E206" s="4"/>
       <c r="F206" s="5"/>
       <c r="G206" s="4"/>
@@ -6778,7 +6635,7 @@
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="4">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B207" s="4"/>
       <c r="E207" s="4"/>
@@ -6788,7 +6645,7 @@
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="4">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B208" s="4"/>
       <c r="C208" s="11"/>
@@ -6799,10 +6656,9 @@
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="4">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B209" s="4"/>
-      <c r="C209" s="11"/>
       <c r="E209" s="4"/>
       <c r="F209" s="5"/>
       <c r="G209" s="4"/>
@@ -6810,9 +6666,10 @@
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="4">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B210" s="4"/>
+      <c r="C210" s="11"/>
       <c r="E210" s="4"/>
       <c r="F210" s="5"/>
       <c r="G210" s="4"/>
@@ -6820,10 +6677,9 @@
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="4">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B211" s="4"/>
-      <c r="C211" s="11"/>
       <c r="E211" s="4"/>
       <c r="F211" s="5"/>
       <c r="G211" s="4"/>
@@ -6831,7 +6687,7 @@
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="4">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B212" s="4"/>
       <c r="E212" s="4"/>
@@ -6841,10 +6697,9 @@
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="4">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B213" s="4"/>
-      <c r="C213" s="11"/>
       <c r="E213" s="4"/>
       <c r="F213" s="5"/>
       <c r="G213" s="4"/>
@@ -6852,7 +6707,7 @@
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="4">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B214" s="4"/>
       <c r="E214" s="4"/>
@@ -6862,7 +6717,7 @@
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="4">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B215" s="4"/>
       <c r="E215" s="4"/>
@@ -6872,7 +6727,7 @@
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="4">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B216" s="4"/>
       <c r="E216" s="4"/>
@@ -6882,7 +6737,7 @@
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="4">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B217" s="4"/>
       <c r="E217" s="4"/>
@@ -6892,7 +6747,7 @@
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="4">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B218" s="4"/>
       <c r="E218" s="4"/>
@@ -6902,7 +6757,7 @@
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="4">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B219" s="4"/>
       <c r="E219" s="4"/>
@@ -6912,7 +6767,7 @@
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="4">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B220" s="4"/>
       <c r="E220" s="4"/>
@@ -6922,7 +6777,7 @@
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="4">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B221" s="4"/>
       <c r="E221" s="4"/>
@@ -6932,7 +6787,7 @@
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="4">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B222" s="4"/>
       <c r="E222" s="4"/>
@@ -6942,7 +6797,7 @@
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="4">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B223" s="4"/>
       <c r="E223" s="4"/>
@@ -6952,18 +6807,17 @@
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="4">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B224" s="4"/>
+      <c r="C224" s="11"/>
       <c r="E224" s="4"/>
       <c r="F224" s="5"/>
       <c r="G224" s="4"/>
       <c r="H224" s="4"/>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A225" s="4">
-        <v>268</v>
-      </c>
+      <c r="A225" s="4"/>
       <c r="B225" s="4"/>
       <c r="E225" s="4"/>
       <c r="F225" s="5"/>
@@ -6971,9 +6825,7 @@
       <c r="H225" s="4"/>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A226" s="4">
-        <v>269</v>
-      </c>
+      <c r="A226" s="4"/>
       <c r="B226" s="4"/>
       <c r="E226" s="4"/>
       <c r="F226" s="5"/>
@@ -6981,11 +6833,8 @@
       <c r="H226" s="4"/>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A227" s="4">
-        <v>270</v>
-      </c>
+      <c r="A227" s="4"/>
       <c r="B227" s="4"/>
-      <c r="C227" s="11"/>
       <c r="E227" s="4"/>
       <c r="F227" s="5"/>
       <c r="G227" s="4"/>
@@ -7262,6 +7111,7 @@
       <c r="F261" s="5"/>
       <c r="G261" s="4"/>
       <c r="H261" s="4"/>
+      <c r="I261" s="4"/>
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" s="4"/>
@@ -7286,7 +7136,6 @@
       <c r="F264" s="5"/>
       <c r="G264" s="4"/>
       <c r="H264" s="4"/>
-      <c r="I264" s="4"/>
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" s="4"/>
@@ -8071,6 +7920,7 @@
       <c r="F362" s="5"/>
       <c r="G362" s="4"/>
       <c r="H362" s="4"/>
+      <c r="I362" s="4"/>
     </row>
     <row r="363" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A363" s="4"/>
@@ -8079,6 +7929,7 @@
       <c r="F363" s="5"/>
       <c r="G363" s="4"/>
       <c r="H363" s="4"/>
+      <c r="I363" s="4"/>
     </row>
     <row r="364" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A364" s="4"/>
@@ -8087,6 +7938,7 @@
       <c r="F364" s="5"/>
       <c r="G364" s="4"/>
       <c r="H364" s="4"/>
+      <c r="I364" s="4"/>
     </row>
     <row r="365" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A365" s="4"/>
@@ -8095,7 +7947,6 @@
       <c r="F365" s="5"/>
       <c r="G365" s="4"/>
       <c r="H365" s="4"/>
-      <c r="I365" s="4"/>
     </row>
     <row r="366" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A366" s="4"/>
@@ -8104,7 +7955,6 @@
       <c r="F366" s="5"/>
       <c r="G366" s="4"/>
       <c r="H366" s="4"/>
-      <c r="I366" s="4"/>
     </row>
     <row r="367" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A367" s="4"/>
@@ -8113,7 +7963,6 @@
       <c r="F367" s="5"/>
       <c r="G367" s="4"/>
       <c r="H367" s="4"/>
-      <c r="I367" s="4"/>
     </row>
     <row r="368" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A368" s="4"/>
@@ -8170,6 +8019,7 @@
       <c r="F374" s="5"/>
       <c r="G374" s="4"/>
       <c r="H374" s="4"/>
+      <c r="I374" s="4"/>
     </row>
     <row r="375" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A375" s="4"/>
@@ -8194,7 +8044,6 @@
       <c r="F377" s="5"/>
       <c r="G377" s="4"/>
       <c r="H377" s="4"/>
-      <c r="I377" s="4"/>
     </row>
     <row r="378" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A378" s="4"/>
@@ -8267,6 +8116,7 @@
       <c r="F386" s="5"/>
       <c r="G386" s="4"/>
       <c r="H386" s="4"/>
+      <c r="I386" s="4"/>
     </row>
     <row r="387" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A387" s="4"/>
@@ -8291,7 +8141,6 @@
       <c r="F389" s="5"/>
       <c r="G389" s="4"/>
       <c r="H389" s="4"/>
-      <c r="I389" s="4"/>
     </row>
     <row r="390" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A390" s="4"/>
@@ -8340,6 +8189,7 @@
       <c r="F395" s="5"/>
       <c r="G395" s="4"/>
       <c r="H395" s="4"/>
+      <c r="I395" s="4"/>
     </row>
     <row r="396" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A396" s="4"/>
@@ -8364,7 +8214,6 @@
       <c r="F398" s="5"/>
       <c r="G398" s="4"/>
       <c r="H398" s="4"/>
-      <c r="I398" s="4"/>
     </row>
     <row r="399" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A399" s="4"/>
@@ -8376,26 +8225,14 @@
     </row>
     <row r="400" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A400" s="4"/>
-      <c r="B400" s="4"/>
-      <c r="E400" s="4"/>
-      <c r="F400" s="5"/>
-      <c r="G400" s="4"/>
       <c r="H400" s="4"/>
     </row>
     <row r="401" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A401" s="4"/>
-      <c r="B401" s="4"/>
-      <c r="E401" s="4"/>
-      <c r="F401" s="5"/>
-      <c r="G401" s="4"/>
       <c r="H401" s="4"/>
     </row>
     <row r="402" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A402" s="4"/>
-      <c r="B402" s="4"/>
-      <c r="E402" s="4"/>
-      <c r="F402" s="5"/>
-      <c r="G402" s="4"/>
       <c r="H402" s="4"/>
     </row>
     <row r="403" spans="1:10" x14ac:dyDescent="0.25">
@@ -8405,28 +8242,28 @@
     <row r="404" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A404" s="4"/>
       <c r="H404" s="4"/>
+      <c r="I404" s="4"/>
+      <c r="J404" s="4"/>
     </row>
     <row r="405" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A405" s="4"/>
-      <c r="H405" s="4"/>
+      <c r="I405" s="4"/>
+      <c r="J405" s="4"/>
     </row>
     <row r="406" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A406" s="4"/>
-      <c r="H406" s="4"/>
+      <c r="I406" s="4"/>
+      <c r="J406" s="4"/>
     </row>
     <row r="407" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A407" s="4"/>
-      <c r="H407" s="4"/>
       <c r="I407" s="4"/>
       <c r="J407" s="4"/>
     </row>
     <row r="408" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A408" s="4"/>
       <c r="I408" s="4"/>
       <c r="J408" s="4"/>
     </row>
     <row r="409" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A409" s="4"/>
       <c r="I409" s="4"/>
       <c r="J409" s="4"/>
     </row>
@@ -8926,24 +8763,11 @@
       <c r="I533" s="4"/>
       <c r="J533" s="4"/>
     </row>
-    <row r="534" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I534" s="4"/>
-      <c r="J534" s="4"/>
-    </row>
-    <row r="535" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I535" s="4"/>
-      <c r="J535" s="4"/>
-    </row>
-    <row r="536" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I536" s="4"/>
-      <c r="J536" s="4"/>
-    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="G2:L2"/>
     <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D16:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>